<commit_message>
Final stage of report
</commit_message>
<xml_diff>
--- a/pythonProject/Results_2/BBvsTime.xlsx
+++ b/pythonProject/Results_2/BBvsTime.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Academic\MSc\Masters Project 2023\Masters-Project-2023\pythonProject\Results_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F6B6C0-B244-4A03-9C02-4A8F7BC64597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F942F3C7-B67E-4FAC-BA57-64A25574E344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{EF9F291A-F117-42A9-906C-9D1655F1BB56}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EF9F291A-F117-42A9-906C-9D1655F1BB56}"/>
   </bookViews>
   <sheets>
     <sheet name="All the results (2)" sheetId="5" r:id="rId1"/>
@@ -87,7 +87,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -120,7 +120,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8015,106 +8015,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:buClrTx/>
-              <a:buSzTx/>
-              <a:buFontTx/>
-              <a:buNone/>
-              <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Process Time vs </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>No. of Neighboring Plant Section Combinations </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.2996955657786656E-2"/>
+          <c:y val="4.0958800771134507E-2"/>
+          <c:w val="0.87451920407534822"/>
+          <c:h val="0.8763775773545095"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -8122,7 +8035,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>1 to 4</c:v>
+            <c:v>1 to 4 Optimized</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -8132,7 +8045,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="plus"/>
             <c:size val="6"/>
             <c:spPr>
               <a:noFill/>
@@ -8207,10 +8120,7 @@
                   <a:pPr>
                     <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
+                        <a:sysClr val="windowText" lastClr="000000"/>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
                       <a:ea typeface="+mn-ea"/>
@@ -8719,7 +8629,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>5 to 9</c:v>
+            <c:v>5 to 9 Optimized</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -8729,13 +8639,13 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="triangle"/>
             <c:size val="6"/>
             <c:spPr>
               <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -8776,10 +8686,7 @@
                   <a:pPr>
                     <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
+                        <a:sysClr val="windowText" lastClr="000000"/>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
                       <a:ea typeface="+mn-ea"/>
@@ -9822,7 +9729,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>10 to 21</c:v>
+            <c:v>10 to 21 Optimized</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -9832,13 +9739,13 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="diamond"/>
             <c:size val="6"/>
             <c:spPr>
               <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -9879,10 +9786,7 @@
                   <a:pPr>
                     <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
+                        <a:sysClr val="windowText" lastClr="000000"/>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
                       <a:ea typeface="+mn-ea"/>
@@ -10337,7 +10241,7 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>0-4 b4</c:v>
+            <c:v>1 to 4</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -10351,11 +10255,9 @@
             <c:size val="6"/>
             <c:spPr>
               <a:noFill/>
-              <a:ln w="0">
+              <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent4">
-                    <a:alpha val="89000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -10396,10 +10298,7 @@
                   <a:pPr>
                     <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
+                        <a:sysClr val="windowText" lastClr="000000"/>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
                       <a:ea typeface="+mn-ea"/>
@@ -10908,7 +10807,7 @@
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>5-9 b4</c:v>
+            <c:v>5 to 9</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -10918,13 +10817,13 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="x"/>
+            <c:symbol val="square"/>
             <c:size val="6"/>
             <c:spPr>
               <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -10965,10 +10864,7 @@
                   <a:pPr>
                     <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
+                        <a:sysClr val="windowText" lastClr="000000"/>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
                       <a:ea typeface="+mn-ea"/>
@@ -12011,7 +11907,7 @@
           <c:idx val="5"/>
           <c:order val="5"/>
           <c:tx>
-            <c:v>10-21 b4</c:v>
+            <c:v>10 to 21</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -12021,13 +11917,13 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="x"/>
+            <c:symbol val="circle"/>
             <c:size val="6"/>
             <c:spPr>
               <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent6"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -12049,8 +11945,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.18780275102563057"/>
-                  <c:y val="-8.381247726875786E-2"/>
+                  <c:x val="-0.18524452380357131"/>
+                  <c:y val="-8.433685015878338E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -12068,10 +11964,7 @@
                   <a:pPr>
                     <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
+                        <a:sysClr val="windowText" lastClr="000000"/>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
                       <a:ea typeface="+mn-ea"/>
@@ -12523,6 +12416,7 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -12543,12 +12437,7 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -12561,7 +12450,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
@@ -12571,7 +12460,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US">
+                  <a:rPr lang="en-US" sz="1100">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
@@ -12579,14 +12468,14 @@
                   <a:t>No.</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0">
+                  <a:rPr lang="en-US" sz="1100" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                   </a:rPr>
                   <a:t> of Neighboring Plant Section Combinations </a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US">
+                <a:endParaRPr lang="en-US" sz="1100">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
@@ -12594,6 +12483,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.38252675483923504"/>
+              <c:y val="0.95775193114492296"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -12607,7 +12504,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
@@ -12621,17 +12518,14 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -12668,12 +12562,7 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -12686,7 +12575,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
@@ -12696,7 +12585,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US">
+                  <a:rPr lang="en-US" sz="1100">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
@@ -12704,14 +12593,14 @@
                   <a:t>Process</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0">
+                  <a:rPr lang="en-US" sz="1100" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                   </a:rPr>
                   <a:t> Time (ms)</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US">
+                <a:endParaRPr lang="en-US" sz="1100">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
@@ -12719,6 +12608,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.7303482494153741E-2"/>
+              <c:y val="0.39419257439563682"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -12732,7 +12629,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
@@ -12746,17 +12643,14 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -12785,12 +12679,84 @@
       </c:valAx>
       <c:spPr>
         <a:noFill/>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="tr"/>
+      <c:legendEntry>
+        <c:idx val="6"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="7"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="8"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="9"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="10"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="11"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="12"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="13"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.82968159861250057"/>
+          <c:y val="6.202918790763276E-2"/>
+          <c:w val="0.12069685827618602"/>
+          <c:h val="0.21709711593423803"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-    </c:plotArea>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -12807,12 +12773,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -12849,72 +12810,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Average Time per Combination vs No. of  Combinations</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
       <c:layout>
         <c:manualLayout>
+          <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.2762532270586448"/>
-          <c:y val="2.4630541871921183E-2"/>
+          <c:x val="0.10177510080261706"/>
+          <c:y val="5.9853408881829682E-2"/>
+          <c:w val="0.85886801513941202"/>
+          <c:h val="0.82931766039974597"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -12935,7 +12843,7 @@
               <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -12960,10 +12868,41 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.25136989457023606"/>
-                  <c:y val="-0.17199970919629021"/>
+                  <c:x val="-0.23598227660872545"/>
+                  <c:y val="-0.13665382344448324"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>T = -167.2ln(N) + 504.12</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US">
+                      <a:solidFill>
+                        <a:sysClr val="windowText" lastClr="000000"/>
+                      </a:solidFill>
+                    </a:endParaRPr>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -12979,10 +12918,7 @@
                   <a:pPr>
                     <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
+                        <a:sysClr val="windowText" lastClr="000000"/>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
                       <a:ea typeface="+mn-ea"/>
@@ -13159,12 +13095,7 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -13177,12 +13108,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -13190,12 +13118,24 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1100" b="1"/>
+                  <a:rPr lang="en-US" sz="1100" b="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t>No. of Combinations</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.43482088516109402"/>
+              <c:y val="0.94651883643299972"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -13209,12 +13149,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -13226,17 +13163,16 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -13247,12 +13183,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -13278,12 +13211,7 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -13296,12 +13224,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -13309,20 +13234,29 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:sysClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                   </a:rPr>
                   <a:t>Average Time per Combination (ms) </a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US" sz="1050" b="1"/>
+                <a:endParaRPr lang="en-US" sz="1100" b="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.2644927536231884E-2"/>
+              <c:y val="0.27530499138251491"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -13336,12 +13270,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -13353,17 +13284,14 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -13374,12 +13302,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -13396,8 +13321,10 @@
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
-          <a:noFill/>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -28684,16 +28611,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>602537</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>60511</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>44823</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>18601</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>130660</xdr:rowOff>
+      <xdr:colOff>89646</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>26894</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -28729,12 +28656,12 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>746760</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>7619</xdr:colOff>
+      <xdr:colOff>541020</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
@@ -29381,8 +29308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58CC68A5-8B63-43E8-A25E-49CA5470C67E}">
   <dimension ref="A1:V317"/>
   <sheetViews>
-    <sheetView topLeftCell="B264" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F311" sqref="F311"/>
+    <sheetView tabSelected="1" topLeftCell="E85" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V34" sqref="V34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29428,7 +29355,7 @@
         <v>1980.9666499975719</v>
       </c>
       <c r="E2">
-        <f>(C2/B2)</f>
+        <f t="shared" ref="E2:E65" si="0">(C2/B2)</f>
         <v>639.02149999921676</v>
       </c>
       <c r="F2">
@@ -29450,7 +29377,7 @@
         <v>2001.0211700041352</v>
       </c>
       <c r="E3">
-        <f>(C3/B3)</f>
+        <f t="shared" si="0"/>
         <v>645.49070000133395</v>
       </c>
     </row>
@@ -29468,7 +29395,7 @@
         <v>2054.5857599999999</v>
       </c>
       <c r="E4">
-        <f>(C4/B4)</f>
+        <f t="shared" si="0"/>
         <v>662.76959999999997</v>
       </c>
     </row>
@@ -29486,7 +29413,7 @@
         <v>2135.1234749996001</v>
       </c>
       <c r="E5">
-        <f>(C5/B5)</f>
+        <f t="shared" si="0"/>
         <v>665.14749999987544</v>
       </c>
     </row>
@@ -29504,7 +29431,7 @@
         <v>2194.7777939919333</v>
       </c>
       <c r="E6">
-        <f>(C6/B6)</f>
+        <f t="shared" si="0"/>
         <v>683.73139999748696</v>
       </c>
     </row>
@@ -29522,7 +29449,7 @@
         <v>2199.567113999401</v>
       </c>
       <c r="E7">
-        <f>(C7/B7)</f>
+        <f t="shared" si="0"/>
         <v>685.22339999981341</v>
       </c>
     </row>
@@ -29540,7 +29467,7 @@
         <v>2177.3420400044415</v>
       </c>
       <c r="E8">
-        <f>(C8/B8)</f>
+        <f t="shared" si="0"/>
         <v>702.36840000143275</v>
       </c>
     </row>
@@ -29558,7 +29485,7 @@
         <v>2197.12345</v>
       </c>
       <c r="E9">
-        <f>(C9/B9)</f>
+        <f t="shared" si="0"/>
         <v>708.74950000000001</v>
       </c>
     </row>
@@ -29576,7 +29503,7 @@
         <v>2217.4997500005702</v>
       </c>
       <c r="E10">
-        <f>(C10/B10)</f>
+        <f t="shared" si="0"/>
         <v>715.32250000018394</v>
       </c>
     </row>
@@ -29594,7 +29521,7 @@
         <v>2300.7071520016179</v>
       </c>
       <c r="E11">
-        <f>(C11/B11)</f>
+        <f t="shared" si="0"/>
         <v>716.73120000050403</v>
       </c>
     </row>
@@ -29612,7 +29539,7 @@
         <v>1990.0356300011119</v>
       </c>
       <c r="E12">
-        <f>(C12/B12)</f>
+        <f t="shared" si="0"/>
         <v>301.5205500001685</v>
       </c>
       <c r="F12">
@@ -29634,7 +29561,7 @@
         <v>2051.1757200032303</v>
       </c>
       <c r="E13">
-        <f>(C13/B13)</f>
+        <f t="shared" si="0"/>
         <v>310.78420000048948</v>
       </c>
     </row>
@@ -29652,7 +29579,7 @@
         <v>1980.1662299999998</v>
       </c>
       <c r="E14">
-        <f>(C14/B14)</f>
+        <f t="shared" si="0"/>
         <v>319.38164999999998</v>
       </c>
     </row>
@@ -29670,7 +29597,7 @@
         <v>2022.1284500020554</v>
       </c>
       <c r="E15">
-        <f>(C15/B15)</f>
+        <f t="shared" si="0"/>
         <v>326.14975000033149</v>
       </c>
     </row>
@@ -29688,7 +29615,7 @@
         <v>2104.3967999983579</v>
       </c>
       <c r="E16">
-        <f>(C16/B16)</f>
+        <f t="shared" si="0"/>
         <v>328.81199999974342</v>
       </c>
     </row>
@@ -29706,7 +29633,7 @@
         <v>2171.7616800000001</v>
       </c>
       <c r="E17">
-        <f>(C17/B17)</f>
+        <f t="shared" si="0"/>
         <v>329.0548</v>
       </c>
     </row>
@@ -29724,7 +29651,7 @@
         <v>2058.3538099977154</v>
       </c>
       <c r="E18">
-        <f>(C18/B18)</f>
+        <f t="shared" si="0"/>
         <v>331.99254999963148</v>
       </c>
     </row>
@@ -29742,7 +29669,7 @@
         <v>2221.8339000002743</v>
       </c>
       <c r="E19">
-        <f>(C19/B19)</f>
+        <f t="shared" si="0"/>
         <v>336.64150000004156</v>
       </c>
     </row>
@@ -29760,7 +29687,7 @@
         <v>2240.4686699999997</v>
       </c>
       <c r="E20">
-        <f>(C20/B20)</f>
+        <f t="shared" si="0"/>
         <v>339.46494999999999</v>
       </c>
     </row>
@@ -29778,7 +29705,7 @@
         <v>2331.4196400000001</v>
       </c>
       <c r="E21">
-        <f>(C21/B21)</f>
+        <f t="shared" si="0"/>
         <v>353.24540000000002</v>
       </c>
     </row>
@@ -29796,7 +29723,7 @@
         <v>2421.1047299997745</v>
       </c>
       <c r="E22">
-        <f>(C22/B22)</f>
+        <f t="shared" si="0"/>
         <v>366.83404999996583</v>
       </c>
     </row>
@@ -29814,7 +29741,7 @@
         <v>2432.1742499923857</v>
       </c>
       <c r="E23">
-        <f>(C23/B23)</f>
+        <f t="shared" si="0"/>
         <v>368.51124999884632</v>
       </c>
     </row>
@@ -29832,7 +29759,7 @@
         <v>2372.7180800051428</v>
       </c>
       <c r="E24">
-        <f>(C24/B24)</f>
+        <f t="shared" si="0"/>
         <v>370.73720000080357</v>
       </c>
     </row>
@@ -29850,7 +29777,7 @@
         <v>2376.7974400077946</v>
       </c>
       <c r="E25">
-        <f>(C25/B25)</f>
+        <f t="shared" si="0"/>
         <v>371.37460000121791</v>
       </c>
     </row>
@@ -29868,7 +29795,7 @@
         <v>2408.1977599998936</v>
       </c>
       <c r="E26">
-        <f>(C26/B26)</f>
+        <f t="shared" si="0"/>
         <v>376.28089999998338</v>
       </c>
     </row>
@@ -29886,7 +29813,7 @@
         <v>2426.115200005006</v>
       </c>
       <c r="E27">
-        <f>(C27/B27)</f>
+        <f t="shared" si="0"/>
         <v>379.08050000078219</v>
       </c>
     </row>
@@ -29904,7 +29831,7 @@
         <v>2622.833279997576</v>
       </c>
       <c r="E28">
-        <f>(C28/B28)</f>
+        <f t="shared" si="0"/>
         <v>409.81769999962125</v>
       </c>
     </row>
@@ -29922,7 +29849,7 @@
         <v>2707.868921999564</v>
       </c>
       <c r="E29">
-        <f>(C29/B29)</f>
+        <f t="shared" si="0"/>
         <v>410.28316999993399</v>
       </c>
     </row>
@@ -29940,7 +29867,7 @@
         <v>2548.0220599987661</v>
       </c>
       <c r="E30">
-        <f>(C30/B30)</f>
+        <f t="shared" si="0"/>
         <v>410.97129999980098</v>
       </c>
     </row>
@@ -29958,7 +29885,7 @@
         <v>2696.1422300008053</v>
       </c>
       <c r="E31">
-        <f>(C31/B31)</f>
+        <f t="shared" si="0"/>
         <v>434.86165000012988</v>
       </c>
     </row>
@@ -29976,7 +29903,7 @@
         <v>2306.5752600003179</v>
       </c>
       <c r="E32">
-        <f>(C32/B32)</f>
+        <f t="shared" si="0"/>
         <v>232.98740000003212</v>
       </c>
       <c r="F32">
@@ -30001,7 +29928,7 @@
         <v>2349.0627600014705</v>
       </c>
       <c r="E33">
-        <f>(C33/B33)</f>
+        <f t="shared" si="0"/>
         <v>237.2790666668152</v>
       </c>
     </row>
@@ -30019,7 +29946,7 @@
         <v>2279.1324799999998</v>
       </c>
       <c r="E34">
-        <f>(C34/B34)</f>
+        <f t="shared" si="0"/>
         <v>237.40963333333332</v>
       </c>
     </row>
@@ -30037,7 +29964,7 @@
         <v>2318.478079992346</v>
       </c>
       <c r="E35">
-        <f>(C35/B35)</f>
+        <f t="shared" si="0"/>
         <v>241.508133332536</v>
       </c>
     </row>
@@ -30055,7 +29982,7 @@
         <v>2416.4088300000003</v>
       </c>
       <c r="E36">
-        <f>(C36/B36)</f>
+        <f t="shared" si="0"/>
         <v>244.08170000000004</v>
       </c>
     </row>
@@ -30073,7 +30000,7 @@
         <v>2354.1193599987309</v>
       </c>
       <c r="E37">
-        <f>(C37/B37)</f>
+        <f t="shared" si="0"/>
         <v>245.22076666653447</v>
       </c>
     </row>
@@ -30091,7 +30018,7 @@
         <v>2368.4320000023586</v>
       </c>
       <c r="E38">
-        <f>(C38/B38)</f>
+        <f t="shared" si="0"/>
         <v>246.71166666691235</v>
       </c>
     </row>
@@ -30109,7 +30036,7 @@
         <v>2407.8399999963585</v>
       </c>
       <c r="E39">
-        <f>(C39/B39)</f>
+        <f t="shared" si="0"/>
         <v>250.81666666628735</v>
       </c>
     </row>
@@ -30127,7 +30054,7 @@
         <v>2413.6015999945812</v>
       </c>
       <c r="E40">
-        <f>(C40/B40)</f>
+        <f t="shared" si="0"/>
         <v>251.41683333276887</v>
       </c>
     </row>
@@ -30145,7 +30072,7 @@
         <v>2472.9043200053252</v>
       </c>
       <c r="E41">
-        <f>(C41/B41)</f>
+        <f t="shared" si="0"/>
         <v>257.59420000055468</v>
       </c>
     </row>
@@ -30163,7 +30090,7 @@
         <v>2475.9635199909098</v>
       </c>
       <c r="E42">
-        <f>(C42/B42)</f>
+        <f t="shared" si="0"/>
         <v>257.91286666571978</v>
       </c>
     </row>
@@ -30181,7 +30108,7 @@
         <v>2616.4678400033154</v>
       </c>
       <c r="E43">
-        <f>(C43/B43)</f>
+        <f t="shared" si="0"/>
         <v>272.54873333367868</v>
       </c>
     </row>
@@ -30199,7 +30126,7 @@
         <v>2740.7030400005169</v>
       </c>
       <c r="E44">
-        <f>(C44/B44)</f>
+        <f t="shared" si="0"/>
         <v>285.48990000005386</v>
       </c>
     </row>
@@ -30217,7 +30144,7 @@
         <v>2801.2294400017709</v>
       </c>
       <c r="E45">
-        <f>(C45/B45)</f>
+        <f t="shared" si="0"/>
         <v>291.7947333335178</v>
       </c>
     </row>
@@ -30235,7 +30162,7 @@
         <v>2851.9081599952187</v>
       </c>
       <c r="E46">
-        <f>(C46/B46)</f>
+        <f t="shared" si="0"/>
         <v>297.07376666616864</v>
       </c>
     </row>
@@ -30253,7 +30180,7 @@
         <v>2865.8774399955291</v>
       </c>
       <c r="E47">
-        <f>(C47/B47)</f>
+        <f t="shared" si="0"/>
         <v>298.5288999995343</v>
       </c>
     </row>
@@ -30271,7 +30198,7 @@
         <v>2218.4547540057247</v>
       </c>
       <c r="E48">
-        <f>(C48/B48)</f>
+        <f t="shared" si="0"/>
         <v>172.77685000044585</v>
       </c>
       <c r="F48">
@@ -30293,7 +30220,7 @@
         <v>2345.7337199957692</v>
       </c>
       <c r="E49">
-        <f>(C49/B49)</f>
+        <f t="shared" si="0"/>
         <v>177.70709999967949</v>
       </c>
     </row>
@@ -30311,7 +30238,7 @@
         <v>2366.858340001636</v>
       </c>
       <c r="E50">
-        <f>(C50/B50)</f>
+        <f t="shared" si="0"/>
         <v>179.30745000012394</v>
       </c>
     </row>
@@ -30329,7 +30256,7 @@
         <v>2399.2336500057718</v>
       </c>
       <c r="E51">
-        <f>(C51/B51)</f>
+        <f t="shared" si="0"/>
         <v>181.76012500043726</v>
       </c>
     </row>
@@ -30347,7 +30274,7 @@
         <v>2406.2458200001856</v>
       </c>
       <c r="E52">
-        <f>(C52/B52)</f>
+        <f t="shared" si="0"/>
         <v>182.29135000001406</v>
       </c>
     </row>
@@ -30365,7 +30292,7 @@
         <v>2434.1199299931759</v>
       </c>
       <c r="E53">
-        <f>(C53/B53)</f>
+        <f t="shared" si="0"/>
         <v>184.40302499948302</v>
       </c>
     </row>
@@ -30383,7 +30310,7 @@
         <v>2497.8538199976897</v>
       </c>
       <c r="E54">
-        <f>(C54/B54)</f>
+        <f t="shared" si="0"/>
         <v>189.231349999825</v>
       </c>
     </row>
@@ -30401,7 +30328,7 @@
         <v>2456.6778419964048</v>
       </c>
       <c r="E55">
-        <f>(C55/B55)</f>
+        <f t="shared" si="0"/>
         <v>191.33004999971999</v>
       </c>
     </row>
@@ -30419,7 +30346,7 @@
         <v>2518.9354709958934</v>
       </c>
       <c r="E56">
-        <f>(C56/B56)</f>
+        <f t="shared" si="0"/>
         <v>196.17877499968017</v>
       </c>
       <c r="V56" s="1"/>
@@ -30438,7 +30365,7 @@
         <v>2537.3756369922639</v>
       </c>
       <c r="E57">
-        <f>(C57/B57)</f>
+        <f t="shared" si="0"/>
         <v>197.61492499939749</v>
       </c>
     </row>
@@ -30456,7 +30383,7 @@
         <v>2571.7662929951257</v>
       </c>
       <c r="E58">
-        <f>(C58/B58)</f>
+        <f t="shared" si="0"/>
         <v>200.29332499962038</v>
       </c>
     </row>
@@ -30474,7 +30401,7 @@
         <v>2653.2438899947529</v>
       </c>
       <c r="E59">
-        <f>(C59/B59)</f>
+        <f t="shared" si="0"/>
         <v>201.00332499960251</v>
       </c>
     </row>
@@ -30492,7 +30419,7 @@
         <v>2592.6579359978859</v>
       </c>
       <c r="E60">
-        <f>(C60/B60)</f>
+        <f t="shared" si="0"/>
         <v>201.92039999983535</v>
       </c>
     </row>
@@ -30510,7 +30437,7 @@
         <v>2604.833144994991</v>
       </c>
       <c r="E61">
-        <f>(C61/B61)</f>
+        <f t="shared" si="0"/>
         <v>202.86862499960989</v>
       </c>
     </row>
@@ -30528,7 +30455,7 @@
         <v>2687.5338600035639</v>
       </c>
       <c r="E62">
-        <f>(C62/B62)</f>
+        <f t="shared" si="0"/>
         <v>203.60105000026999</v>
       </c>
     </row>
@@ -30546,7 +30473,7 @@
         <v>2651.7954449960198</v>
       </c>
       <c r="E63">
-        <f>(C63/B63)</f>
+        <f t="shared" si="0"/>
         <v>206.52612499969001</v>
       </c>
     </row>
@@ -30564,7 +30491,7 @@
         <v>2736.1827899980526</v>
       </c>
       <c r="E64">
-        <f>(C64/B64)</f>
+        <f t="shared" si="0"/>
         <v>207.28657499985249</v>
       </c>
     </row>
@@ -30582,7 +30509,7 @@
         <v>2749.5817800032669</v>
       </c>
       <c r="E65">
-        <f>(C65/B65)</f>
+        <f t="shared" si="0"/>
         <v>208.30165000024749</v>
       </c>
     </row>
@@ -30600,7 +30527,7 @@
         <v>2680.8623159978015</v>
       </c>
       <c r="E66">
-        <f>(C66/B66)</f>
+        <f t="shared" ref="E66:E129" si="1">(C66/B66)</f>
         <v>208.78989999982878</v>
       </c>
     </row>
@@ -30618,7 +30545,7 @@
         <v>2763.9008099982179</v>
       </c>
       <c r="E67">
-        <f>(C67/B67)</f>
+        <f t="shared" si="1"/>
         <v>209.386424999865</v>
       </c>
     </row>
@@ -30636,7 +30563,7 @@
         <v>2713.4248769997794</v>
       </c>
       <c r="E68">
-        <f>(C68/B68)</f>
+        <f t="shared" si="1"/>
         <v>211.32592499998282</v>
       </c>
     </row>
@@ -30654,7 +30581,7 @@
         <v>2881.9253400099115</v>
       </c>
       <c r="E69">
-        <f>(C69/B69)</f>
+        <f t="shared" si="1"/>
         <v>211.90627500072878</v>
       </c>
     </row>
@@ -30672,7 +30599,7 @@
         <v>2883.5491799931333</v>
       </c>
       <c r="E70">
-        <f>(C70/B70)</f>
+        <f t="shared" si="1"/>
         <v>212.0256749994951</v>
       </c>
     </row>
@@ -30690,7 +30617,7 @@
         <v>2921.7838799988385</v>
       </c>
       <c r="E71">
-        <f>(C71/B71)</f>
+        <f t="shared" si="1"/>
         <v>214.8370499999146</v>
       </c>
     </row>
@@ -30708,7 +30635,7 @@
         <v>2936.4895599974261</v>
       </c>
       <c r="E72">
-        <f>(C72/B72)</f>
+        <f t="shared" si="1"/>
         <v>215.91834999981074</v>
       </c>
     </row>
@@ -30726,7 +30653,7 @@
         <v>2890.3177380000757</v>
       </c>
       <c r="E73">
-        <f>(C73/B73)</f>
+        <f t="shared" si="1"/>
         <v>218.96346500000575</v>
       </c>
     </row>
@@ -30744,7 +30671,7 @@
         <v>2981.2182599998778</v>
       </c>
       <c r="E74">
-        <f>(C74/B74)</f>
+        <f t="shared" si="1"/>
         <v>219.20722499999101</v>
       </c>
     </row>
@@ -30762,7 +30689,7 @@
         <v>2821.5103919990206</v>
       </c>
       <c r="E75">
-        <f>(C75/B75)</f>
+        <f t="shared" si="1"/>
         <v>219.74379999992374</v>
       </c>
     </row>
@@ -30780,7 +30707,7 @@
         <v>2917.3828200079197</v>
       </c>
       <c r="E76">
-        <f>(C76/B76)</f>
+        <f t="shared" si="1"/>
         <v>221.0138500006</v>
       </c>
     </row>
@@ -30798,7 +30725,7 @@
         <v>2951.0240100036035</v>
       </c>
       <c r="E77">
-        <f>(C77/B77)</f>
+        <f t="shared" si="1"/>
         <v>223.56242500027301</v>
       </c>
     </row>
@@ -30816,7 +30743,7 @@
         <v>3020.1866009955847</v>
       </c>
       <c r="E78">
-        <f>(C78/B78)</f>
+        <f t="shared" si="1"/>
         <v>235.21702499965613</v>
       </c>
     </row>
@@ -30834,7 +30761,7 @@
         <v>3117.0213870000589</v>
       </c>
       <c r="E79">
-        <f>(C79/B79)</f>
+        <f t="shared" si="1"/>
         <v>242.75867500000459</v>
       </c>
     </row>
@@ -30852,7 +30779,7 @@
         <v>2420.0075403000769</v>
       </c>
       <c r="E80">
-        <f>(C80/B80)</f>
+        <f t="shared" si="1"/>
         <v>150.77928600000479</v>
       </c>
       <c r="F80">
@@ -30874,7 +30801,7 @@
         <v>2437.7600280037404</v>
       </c>
       <c r="E81">
-        <f>(C81/B81)</f>
+        <f t="shared" si="1"/>
         <v>151.88536000023305</v>
       </c>
     </row>
@@ -30892,7 +30819,7 @@
         <v>2523.1031099999996</v>
       </c>
       <c r="E82">
-        <f>(C82/B82)</f>
+        <f t="shared" si="1"/>
         <v>152.91533999999999</v>
       </c>
     </row>
@@ -30910,7 +30837,7 @@
         <v>2479.7404079977423</v>
       </c>
       <c r="E83">
-        <f>(C83/B83)</f>
+        <f t="shared" si="1"/>
         <v>154.50095999985933</v>
       </c>
     </row>
@@ -30928,7 +30855,7 @@
         <v>2538.3517979990211</v>
       </c>
       <c r="E84">
-        <f>(C84/B84)</f>
+        <f t="shared" si="1"/>
         <v>158.15275999993901</v>
       </c>
     </row>
@@ -30946,7 +30873,7 @@
         <v>2589.6918960000003</v>
       </c>
       <c r="E85">
-        <f>(C85/B85)</f>
+        <f t="shared" si="1"/>
         <v>161.35151999999999</v>
       </c>
     </row>
@@ -30964,7 +30891,7 @@
         <v>2676.3537899999997</v>
       </c>
       <c r="E86">
-        <f>(C86/B86)</f>
+        <f t="shared" si="1"/>
         <v>162.20326</v>
       </c>
     </row>
@@ -30982,7 +30909,7 @@
         <v>2628.6352950067885</v>
       </c>
       <c r="E87">
-        <f>(C87/B87)</f>
+        <f t="shared" si="1"/>
         <v>163.77790000042296</v>
       </c>
     </row>
@@ -31000,7 +30927,7 @@
         <v>2676.5063460062447</v>
       </c>
       <c r="E88">
-        <f>(C88/B88)</f>
+        <f t="shared" si="1"/>
         <v>166.76052000038908</v>
       </c>
     </row>
@@ -31018,7 +30945,7 @@
         <v>2690.416559997464</v>
       </c>
       <c r="E89">
-        <f>(C89/B89)</f>
+        <f t="shared" si="1"/>
         <v>167.62719999984199</v>
       </c>
     </row>
@@ -31036,7 +30963,7 @@
         <v>2690.5728869943414</v>
       </c>
       <c r="E90">
-        <f>(C90/B90)</f>
+        <f t="shared" si="1"/>
         <v>167.63693999964744</v>
       </c>
     </row>
@@ -31054,7 +30981,7 @@
         <v>2868.8768199946935</v>
       </c>
       <c r="E91">
-        <f>(C91/B91)</f>
+        <f t="shared" si="1"/>
         <v>168.75745999968785</v>
       </c>
     </row>
@@ -31072,7 +30999,7 @@
         <v>2937.1760200046992</v>
       </c>
       <c r="E92">
-        <f>(C92/B92)</f>
+        <f t="shared" si="1"/>
         <v>172.77506000027643</v>
       </c>
     </row>
@@ -31090,7 +31017,7 @@
         <v>2868.6091499999998</v>
       </c>
       <c r="E93">
-        <f>(C93/B93)</f>
+        <f t="shared" si="1"/>
         <v>173.85509999999999</v>
       </c>
     </row>
@@ -31108,7 +31035,7 @@
         <v>2957.2567599972526</v>
       </c>
       <c r="E94">
-        <f>(C94/B94)</f>
+        <f t="shared" si="1"/>
         <v>173.95627999983839</v>
       </c>
     </row>
@@ -31126,7 +31053,7 @@
         <v>2923.7003399966998</v>
       </c>
       <c r="E95">
-        <f>(C95/B95)</f>
+        <f t="shared" si="1"/>
         <v>177.1939599998</v>
       </c>
     </row>
@@ -31144,7 +31071,7 @@
         <v>2846.7403500046544</v>
       </c>
       <c r="E96">
-        <f>(C96/B96)</f>
+        <f t="shared" si="1"/>
         <v>177.36700000029001</v>
       </c>
     </row>
@@ -31162,7 +31089,7 @@
         <v>2849.6771790000003</v>
       </c>
       <c r="E97">
-        <f>(C97/B97)</f>
+        <f t="shared" si="1"/>
         <v>177.54998000000001</v>
       </c>
     </row>
@@ -31180,7 +31107,7 @@
         <v>2933.463719999043</v>
       </c>
       <c r="E98">
-        <f>(C98/B98)</f>
+        <f t="shared" si="1"/>
         <v>177.785679999942</v>
       </c>
     </row>
@@ -31198,7 +31125,7 @@
         <v>3009.3346799999995</v>
       </c>
       <c r="E99">
-        <f>(C99/B99)</f>
+        <f t="shared" si="1"/>
         <v>182.38391999999999</v>
       </c>
     </row>
@@ -31216,7 +31143,7 @@
         <v>3112.7265200011607</v>
       </c>
       <c r="E100">
-        <f>(C100/B100)</f>
+        <f t="shared" si="1"/>
         <v>183.10156000006828</v>
       </c>
     </row>
@@ -31234,7 +31161,7 @@
         <v>3135.2559399914762</v>
       </c>
       <c r="E101">
-        <f>(C101/B101)</f>
+        <f t="shared" si="1"/>
         <v>184.4268199994986</v>
       </c>
     </row>
@@ -31252,7 +31179,7 @@
         <v>2383.9192199980162</v>
       </c>
       <c r="E102">
-        <f>(C102/B102)</f>
+        <f t="shared" si="1"/>
         <v>128.16769999989333</v>
       </c>
       <c r="F102">
@@ -31275,7 +31202,7 @@
         <v>2494.7622400010005</v>
       </c>
       <c r="E103">
-        <f>(C103/B103)</f>
+        <f t="shared" si="1"/>
         <v>129.93553333338545</v>
       </c>
     </row>
@@ -31293,7 +31220,7 @@
         <v>2511.2642130082177</v>
       </c>
       <c r="E104">
-        <f>(C104/B104)</f>
+        <f t="shared" si="1"/>
         <v>130.38755000042667</v>
       </c>
     </row>
@@ -31311,7 +31238,7 @@
         <v>2507.9023999976926</v>
       </c>
       <c r="E105">
-        <f>(C105/B105)</f>
+        <f t="shared" si="1"/>
         <v>130.61991666654649</v>
       </c>
     </row>
@@ -31329,7 +31256,7 @@
         <v>2436.0032500080601</v>
       </c>
       <c r="E106">
-        <f>(C106/B106)</f>
+        <f t="shared" si="1"/>
         <v>130.96791666710001</v>
       </c>
     </row>
@@ -31347,7 +31274,7 @@
         <v>2447.370640005332</v>
       </c>
       <c r="E107">
-        <f>(C107/B107)</f>
+        <f t="shared" si="1"/>
         <v>131.57906666695334</v>
       </c>
     </row>
@@ -31365,7 +31292,7 @@
         <v>2535.4233150040768</v>
       </c>
       <c r="E108">
-        <f>(C108/B108)</f>
+        <f t="shared" si="1"/>
         <v>131.64191666687833</v>
       </c>
     </row>
@@ -31383,7 +31310,7 @@
         <v>2565.2543999953195</v>
       </c>
       <c r="E109">
-        <f>(C109/B109)</f>
+        <f t="shared" si="1"/>
         <v>133.60699999975623</v>
       </c>
     </row>
@@ -31401,7 +31328,7 @@
         <v>2656.7828099958419</v>
       </c>
       <c r="E110">
-        <f>(C110/B110)</f>
+        <f t="shared" si="1"/>
         <v>134.18094999978999</v>
       </c>
     </row>
@@ -31419,7 +31346,7 @@
         <v>2699.844510011319</v>
       </c>
       <c r="E111">
-        <f>(C111/B111)</f>
+        <f t="shared" si="1"/>
         <v>136.35578333390501</v>
       </c>
     </row>
@@ -31437,7 +31364,7 @@
         <v>2621.8886399990879</v>
       </c>
       <c r="E112">
-        <f>(C112/B112)</f>
+        <f t="shared" si="1"/>
         <v>136.55669999995249</v>
       </c>
     </row>
@@ -31455,7 +31382,7 @@
         <v>2635.7312000007369</v>
       </c>
       <c r="E113">
-        <f>(C113/B113)</f>
+        <f t="shared" si="1"/>
         <v>137.27766666670504</v>
       </c>
     </row>
@@ -31473,7 +31400,7 @@
         <v>2665.9014690012195</v>
       </c>
       <c r="E114">
-        <f>(C114/B114)</f>
+        <f t="shared" si="1"/>
         <v>138.41648333339666</v>
       </c>
     </row>
@@ -31491,7 +31418,7 @@
         <v>2590.709989998868</v>
       </c>
       <c r="E115">
-        <f>(C115/B115)</f>
+        <f t="shared" si="1"/>
         <v>139.28548333327248</v>
       </c>
     </row>
@@ -31509,7 +31436,7 @@
         <v>2592.110880001705</v>
       </c>
       <c r="E116">
-        <f>(C116/B116)</f>
+        <f t="shared" si="1"/>
         <v>139.36080000009167</v>
       </c>
     </row>
@@ -31527,7 +31454,7 @@
         <v>2650.4345899999998</v>
       </c>
       <c r="E117">
-        <f>(C117/B117)</f>
+        <f t="shared" si="1"/>
         <v>142.49648333333332</v>
       </c>
     </row>
@@ -31545,7 +31472,7 @@
         <v>2696.6701600000001</v>
       </c>
       <c r="E118">
-        <f>(C118/B118)</f>
+        <f t="shared" si="1"/>
         <v>144.98226666666667</v>
       </c>
     </row>
@@ -31563,7 +31490,7 @@
         <v>2876.5512599983167</v>
       </c>
       <c r="E119">
-        <f>(C119/B119)</f>
+        <f t="shared" si="1"/>
         <v>145.28036666658167</v>
       </c>
     </row>
@@ -31581,7 +31508,7 @@
         <v>2706.7826699995976</v>
       </c>
       <c r="E120">
-        <f>(C120/B120)</f>
+        <f t="shared" si="1"/>
         <v>145.52594999997837</v>
       </c>
     </row>
@@ -31599,7 +31526,7 @@
         <v>2710.9323299970861</v>
       </c>
       <c r="E121">
-        <f>(C121/B121)</f>
+        <f t="shared" si="1"/>
         <v>145.74904999984332</v>
       </c>
     </row>
@@ -31617,7 +31544,7 @@
         <v>2763.870100002604</v>
       </c>
       <c r="E122">
-        <f>(C122/B122)</f>
+        <f t="shared" si="1"/>
         <v>148.59516666680665</v>
       </c>
     </row>
@@ -31635,7 +31562,7 @@
         <v>2871.1190159993257</v>
       </c>
       <c r="E123">
-        <f>(C123/B123)</f>
+        <f t="shared" si="1"/>
         <v>149.071599999965</v>
       </c>
     </row>
@@ -31653,7 +31580,7 @@
         <v>2969.6865000067191</v>
       </c>
       <c r="E124">
-        <f>(C124/B124)</f>
+        <f t="shared" si="1"/>
         <v>149.98416666700601</v>
       </c>
     </row>
@@ -31671,7 +31598,7 @@
         <v>3033.0824700005905</v>
       </c>
       <c r="E125">
-        <f>(C125/B125)</f>
+        <f t="shared" si="1"/>
         <v>153.18598333336317</v>
       </c>
     </row>
@@ -31689,7 +31616,7 @@
         <v>3045.2056800037099</v>
       </c>
       <c r="E126">
-        <f>(C126/B126)</f>
+        <f t="shared" si="1"/>
         <v>153.79826666685403</v>
       </c>
     </row>
@@ -31707,7 +31634,7 @@
         <v>3027.2113800000002</v>
       </c>
       <c r="E127">
-        <f>(C127/B127)</f>
+        <f t="shared" si="1"/>
         <v>162.7533</v>
       </c>
     </row>
@@ -31725,7 +31652,7 @@
         <v>2552.5087999994867</v>
       </c>
       <c r="E128">
-        <f>(C128/B128)</f>
+        <f t="shared" si="1"/>
         <v>113.9512857142628</v>
       </c>
       <c r="F128">
@@ -31747,7 +31674,7 @@
         <v>2656.3657599966973</v>
       </c>
       <c r="E129">
-        <f>(C129/B129)</f>
+        <f t="shared" si="1"/>
         <v>118.58775714270971</v>
       </c>
     </row>
@@ -31765,7 +31692,7 @@
         <v>2694.2911999998614</v>
       </c>
       <c r="E130">
-        <f>(C130/B130)</f>
+        <f t="shared" ref="E130:E193" si="2">(C130/B130)</f>
         <v>120.28085714285096</v>
       </c>
     </row>
@@ -31783,7 +31710,7 @@
         <v>2875.4243200004566</v>
       </c>
       <c r="E131">
-        <f>(C131/B131)</f>
+        <f t="shared" si="2"/>
         <v>128.36715714287752</v>
       </c>
     </row>
@@ -31801,7 +31728,7 @@
         <v>2997.314430005214</v>
       </c>
       <c r="E132">
-        <f>(C132/B132)</f>
+        <f t="shared" si="2"/>
         <v>129.75387142879714</v>
       </c>
     </row>
@@ -31819,7 +31746,7 @@
         <v>2822.5450399993179</v>
       </c>
       <c r="E133">
-        <f>(C133/B133)</f>
+        <f t="shared" si="2"/>
         <v>130.07119999996857</v>
       </c>
     </row>
@@ -31837,7 +31764,7 @@
         <v>2837.4572800000001</v>
       </c>
       <c r="E134">
-        <f>(C134/B134)</f>
+        <f t="shared" si="2"/>
         <v>130.75839999999999</v>
       </c>
     </row>
@@ -31855,7 +31782,7 @@
         <v>3049.7821199995087</v>
       </c>
       <c r="E135">
-        <f>(C135/B135)</f>
+        <f t="shared" si="2"/>
         <v>132.02519999997872</v>
       </c>
     </row>
@@ -31873,7 +31800,7 @@
         <v>3053.7365100080187</v>
       </c>
       <c r="E136">
-        <f>(C136/B136)</f>
+        <f t="shared" si="2"/>
         <v>132.19638571463287</v>
       </c>
     </row>
@@ -31891,7 +31818,7 @@
         <v>3072.0317099996464</v>
       </c>
       <c r="E137">
-        <f>(C137/B137)</f>
+        <f t="shared" si="2"/>
         <v>132.98838571427041</v>
       </c>
     </row>
@@ -31909,7 +31836,7 @@
         <v>3088.0964399925087</v>
       </c>
       <c r="E138">
-        <f>(C138/B138)</f>
+        <f t="shared" si="2"/>
         <v>133.68382857110427</v>
       </c>
     </row>
@@ -31927,7 +31854,7 @@
         <v>3089.9579699984315</v>
       </c>
       <c r="E139">
-        <f>(C139/B139)</f>
+        <f t="shared" si="2"/>
         <v>133.76441428564638</v>
       </c>
     </row>
@@ -31945,7 +31872,7 @@
         <v>3004.9715199973434</v>
       </c>
       <c r="E140">
-        <f>(C140/B140)</f>
+        <f t="shared" si="2"/>
         <v>134.15051428559568</v>
       </c>
     </row>
@@ -31963,7 +31890,7 @@
         <v>3113.5216200004288</v>
       </c>
       <c r="E141">
-        <f>(C141/B141)</f>
+        <f t="shared" si="2"/>
         <v>134.78448571430428</v>
       </c>
     </row>
@@ -31981,7 +31908,7 @@
         <v>3023.4803200000897</v>
       </c>
       <c r="E142">
-        <f>(C142/B142)</f>
+        <f t="shared" si="2"/>
         <v>134.976800000004</v>
       </c>
     </row>
@@ -31999,7 +31926,7 @@
         <v>3028.6281600012444</v>
       </c>
       <c r="E143">
-        <f>(C143/B143)</f>
+        <f t="shared" si="2"/>
         <v>135.20661428576983</v>
       </c>
     </row>
@@ -32017,7 +31944,7 @@
         <v>2938.3619699947922</v>
       </c>
       <c r="E144">
-        <f>(C144/B144)</f>
+        <f t="shared" si="2"/>
         <v>135.40838571404572</v>
       </c>
     </row>
@@ -32035,7 +31962,7 @@
         <v>2954.6372799920332</v>
       </c>
       <c r="E145">
-        <f>(C145/B145)</f>
+        <f t="shared" si="2"/>
         <v>136.15839999963285</v>
       </c>
     </row>
@@ -32053,7 +31980,7 @@
         <v>2956.6916499999998</v>
       </c>
       <c r="E146">
-        <f>(C146/B146)</f>
+        <f t="shared" si="2"/>
         <v>136.25307142857142</v>
       </c>
     </row>
@@ -32071,7 +31998,7 @@
         <v>3056.1907199968118</v>
       </c>
       <c r="E147">
-        <f>(C147/B147)</f>
+        <f t="shared" si="2"/>
         <v>136.43708571414339</v>
       </c>
     </row>
@@ -32089,7 +32016,7 @@
         <v>2961.0239000000001</v>
       </c>
       <c r="E148">
-        <f>(C148/B148)</f>
+        <f t="shared" si="2"/>
         <v>136.45271428571428</v>
       </c>
     </row>
@@ -32107,7 +32034,7 @@
         <v>3075.4278120050394</v>
       </c>
       <c r="E149">
-        <f>(C149/B149)</f>
+        <f t="shared" si="2"/>
         <v>136.8681714287957</v>
       </c>
     </row>
@@ -32125,7 +32052,7 @@
         <v>3173.7297899943896</v>
       </c>
       <c r="E150">
-        <f>(C150/B150)</f>
+        <f t="shared" si="2"/>
         <v>137.39089999975712</v>
       </c>
     </row>
@@ -32143,7 +32070,7 @@
         <v>3086.8262399977539</v>
       </c>
       <c r="E151">
-        <f>(C151/B151)</f>
+        <f t="shared" si="2"/>
         <v>137.80474285704258</v>
       </c>
     </row>
@@ -32161,7 +32088,7 @@
         <v>2997.5074900087111</v>
       </c>
       <c r="E152">
-        <f>(C152/B152)</f>
+        <f t="shared" si="2"/>
         <v>138.13398571468716</v>
       </c>
     </row>
@@ -32179,7 +32106,7 @@
         <v>3005.430160004471</v>
       </c>
       <c r="E153">
-        <f>(C153/B153)</f>
+        <f t="shared" si="2"/>
         <v>138.49908571449174</v>
       </c>
     </row>
@@ -32197,7 +32124,7 @@
         <v>3018.833630001609</v>
       </c>
       <c r="E154">
-        <f>(C154/B154)</f>
+        <f t="shared" si="2"/>
         <v>139.11675714293128</v>
       </c>
     </row>
@@ -32215,7 +32142,7 @@
         <v>3151.7930699978492</v>
       </c>
       <c r="E155">
-        <f>(C155/B155)</f>
+        <f t="shared" si="2"/>
         <v>140.26671428561858</v>
       </c>
     </row>
@@ -32233,7 +32160,7 @@
         <v>3045.5029300034103</v>
       </c>
       <c r="E156">
-        <f>(C156/B156)</f>
+        <f t="shared" si="2"/>
         <v>140.34575714301428</v>
       </c>
     </row>
@@ -32251,7 +32178,7 @@
         <v>3260.0228100083159</v>
       </c>
       <c r="E157">
-        <f>(C157/B157)</f>
+        <f t="shared" si="2"/>
         <v>141.12652857178858</v>
       </c>
     </row>
@@ -32269,7 +32196,7 @@
         <v>3183.1891169996147</v>
       </c>
       <c r="E158">
-        <f>(C158/B158)</f>
+        <f t="shared" si="2"/>
         <v>141.66395714284002</v>
       </c>
     </row>
@@ -32287,7 +32214,7 @@
         <v>3197.8122719986518</v>
       </c>
       <c r="E159">
-        <f>(C159/B159)</f>
+        <f t="shared" si="2"/>
         <v>142.31474285708285</v>
       </c>
     </row>
@@ -32305,7 +32232,7 @@
         <v>3092.0401299984192</v>
       </c>
       <c r="E160">
-        <f>(C160/B160)</f>
+        <f t="shared" si="2"/>
         <v>142.49032857135572</v>
       </c>
     </row>
@@ -32323,7 +32250,7 @@
         <v>2795.5564007934227</v>
       </c>
       <c r="E161">
-        <f>(C161/B161)</f>
+        <f t="shared" si="2"/>
         <v>106.47304999974949</v>
       </c>
       <c r="F161">
@@ -32345,7 +32272,7 @@
         <v>2807.2629666020366</v>
       </c>
       <c r="E162">
-        <f>(C162/B162)</f>
+        <f t="shared" si="2"/>
         <v>106.91891250007757</v>
       </c>
     </row>
@@ -32363,7 +32290,7 @@
         <v>2810.743199401757</v>
       </c>
       <c r="E163">
-        <f>(C163/B163)</f>
+        <f t="shared" si="2"/>
         <v>107.05146250006692</v>
       </c>
     </row>
@@ -32381,7 +32308,7 @@
         <v>2855.1191213982966</v>
       </c>
       <c r="E164">
-        <f>(C164/B164)</f>
+        <f t="shared" si="2"/>
         <v>108.74158749993512</v>
       </c>
     </row>
@@ -32399,7 +32326,7 @@
         <v>2715.6526122333307</v>
       </c>
       <c r="E165">
-        <f>(C165/B165)</f>
+        <f t="shared" si="2"/>
         <v>109.4197625</v>
       </c>
     </row>
@@ -32417,7 +32344,7 @@
         <v>2894.9478324016527</v>
       </c>
       <c r="E166">
-        <f>(C166/B166)</f>
+        <f t="shared" si="2"/>
         <v>110.25852500006295</v>
       </c>
     </row>
@@ -32435,7 +32362,7 @@
         <v>2947.4801808001357</v>
       </c>
       <c r="E167">
-        <f>(C167/B167)</f>
+        <f t="shared" si="2"/>
         <v>112.25930000000517</v>
       </c>
     </row>
@@ -32453,7 +32380,7 @@
         <v>2787.5628374999969</v>
       </c>
       <c r="E168">
-        <f>(C168/B168)</f>
+        <f t="shared" si="2"/>
         <v>112.3171875</v>
       </c>
     </row>
@@ -32471,7 +32398,7 @@
         <v>2978.2364591958976</v>
       </c>
       <c r="E169">
-        <f>(C169/B169)</f>
+        <f t="shared" si="2"/>
         <v>113.43069999984375</v>
       </c>
     </row>
@@ -32489,7 +32416,7 @@
         <v>3021.3892499989765</v>
       </c>
       <c r="E170">
-        <f>(C170/B170)</f>
+        <f t="shared" si="2"/>
         <v>114.44656249996125</v>
       </c>
     </row>
@@ -32507,7 +32434,7 @@
         <v>3032.1178799993727</v>
       </c>
       <c r="E171">
-        <f>(C171/B171)</f>
+        <f t="shared" si="2"/>
         <v>114.85294999997625</v>
       </c>
     </row>
@@ -32525,7 +32452,7 @@
         <v>3017.5436604018178</v>
       </c>
       <c r="E172">
-        <f>(C172/B172)</f>
+        <f t="shared" si="2"/>
         <v>114.92777500006923</v>
       </c>
     </row>
@@ -32543,7 +32470,7 @@
         <v>3044.866966791189</v>
       </c>
       <c r="E173">
-        <f>(C173/B173)</f>
+        <f t="shared" si="2"/>
         <v>115.96842499966442</v>
       </c>
     </row>
@@ -32561,7 +32488,7 @@
         <v>3052.4953194018162</v>
       </c>
       <c r="E174">
-        <f>(C174/B174)</f>
+        <f t="shared" si="2"/>
         <v>116.25896250006917</v>
       </c>
     </row>
@@ -32579,7 +32506,7 @@
         <v>3071.5297799977889</v>
       </c>
       <c r="E175">
-        <f>(C175/B175)</f>
+        <f t="shared" si="2"/>
         <v>116.34582499991625</v>
       </c>
     </row>
@@ -32597,7 +32524,7 @@
         <v>3077.585609997393</v>
       </c>
       <c r="E176">
-        <f>(C176/B176)</f>
+        <f t="shared" si="2"/>
         <v>116.57521249990126</v>
       </c>
     </row>
@@ -32615,7 +32542,7 @@
         <v>3097.8348365986094</v>
       </c>
       <c r="E177">
-        <f>(C177/B177)</f>
+        <f t="shared" si="2"/>
         <v>117.98578749994704</v>
       </c>
     </row>
@@ -32633,7 +32560,7 @@
         <v>2942.8302775666634</v>
       </c>
       <c r="E178">
-        <f>(C178/B178)</f>
+        <f t="shared" si="2"/>
         <v>118.5732625</v>
       </c>
     </row>
@@ -32651,7 +32578,7 @@
         <v>3132.3148722000001</v>
       </c>
       <c r="E179">
-        <f>(C179/B179)</f>
+        <f t="shared" si="2"/>
         <v>119.2990125</v>
       </c>
     </row>
@@ -32669,7 +32596,7 @@
         <v>3159.2163899984821</v>
       </c>
       <c r="E180">
-        <f>(C180/B180)</f>
+        <f t="shared" si="2"/>
         <v>119.6672874999425</v>
       </c>
     </row>
@@ -32687,7 +32614,7 @@
         <v>2976.4629834666634</v>
       </c>
       <c r="E181">
-        <f>(C181/B181)</f>
+        <f t="shared" si="2"/>
         <v>119.9284</v>
       </c>
     </row>
@@ -32705,7 +32632,7 @@
         <v>3149.9129562009257</v>
       </c>
       <c r="E182">
-        <f>(C182/B182)</f>
+        <f t="shared" si="2"/>
         <v>119.96926250003526</v>
       </c>
     </row>
@@ -32723,7 +32650,7 @@
         <v>3161.4941495981402</v>
       </c>
       <c r="E183">
-        <f>(C183/B183)</f>
+        <f t="shared" si="2"/>
         <v>120.41034999992917</v>
       </c>
     </row>
@@ -32741,7 +32668,7 @@
         <v>3029.399958537022</v>
       </c>
       <c r="E184">
-        <f>(C184/B184)</f>
+        <f t="shared" si="2"/>
         <v>122.06135000014875</v>
       </c>
     </row>
@@ -32759,7 +32686,7 @@
         <v>3213.6044328065691</v>
       </c>
       <c r="E185">
-        <f>(C185/B185)</f>
+        <f t="shared" si="2"/>
         <v>122.39505000025019</v>
       </c>
     </row>
@@ -32777,7 +32704,7 @@
         <v>3220.4575770007214</v>
       </c>
       <c r="E186">
-        <f>(C186/B186)</f>
+        <f t="shared" si="2"/>
         <v>122.65606250002747</v>
       </c>
     </row>
@@ -32795,7 +32722,7 @@
         <v>3265.8416999949177</v>
       </c>
       <c r="E187">
-        <f>(C187/B187)</f>
+        <f t="shared" si="2"/>
         <v>123.7061249998075</v>
       </c>
     </row>
@@ -32813,7 +32740,7 @@
         <v>3285.452940002277</v>
       </c>
       <c r="E188">
-        <f>(C188/B188)</f>
+        <f t="shared" si="2"/>
         <v>124.44897500008625</v>
       </c>
     </row>
@@ -32831,7 +32758,7 @@
         <v>3296.4769020056124</v>
       </c>
       <c r="E189">
-        <f>(C189/B189)</f>
+        <f t="shared" si="2"/>
         <v>125.55137500021375</v>
       </c>
     </row>
@@ -32849,7 +32776,7 @@
         <v>3247.2806189970147</v>
       </c>
       <c r="E190">
-        <f>(C190/B190)</f>
+        <f t="shared" si="2"/>
         <v>126.45173749988375</v>
       </c>
     </row>
@@ -32867,7 +32794,7 @@
         <v>3283.6820189999676</v>
       </c>
       <c r="E191">
-        <f>(C191/B191)</f>
+        <f t="shared" si="2"/>
         <v>127.86923749999875</v>
       </c>
     </row>
@@ -32885,7 +32812,7 @@
         <v>3376.4582574013948</v>
       </c>
       <c r="E192">
-        <f>(C192/B192)</f>
+        <f t="shared" si="2"/>
         <v>128.59758750005312</v>
       </c>
     </row>
@@ -32903,7 +32830,7 @@
         <v>3326.204247003403</v>
       </c>
       <c r="E193">
-        <f>(C193/B193)</f>
+        <f t="shared" si="2"/>
         <v>129.52508750013251</v>
       </c>
     </row>
@@ -32921,7 +32848,7 @@
         <v>3426.2839404041356</v>
       </c>
       <c r="E194">
-        <f>(C194/B194)</f>
+        <f t="shared" ref="E194:E257" si="3">(C194/B194)</f>
         <v>130.49527500015751</v>
       </c>
     </row>
@@ -32939,7 +32866,7 @@
         <v>3435.1440275971413</v>
       </c>
       <c r="E195">
-        <f>(C195/B195)</f>
+        <f t="shared" si="3"/>
         <v>130.83272499989113</v>
       </c>
     </row>
@@ -32957,7 +32884,7 @@
         <v>3464.9161799980197</v>
       </c>
       <c r="E196">
-        <f>(C196/B196)</f>
+        <f t="shared" si="3"/>
         <v>131.246824999925</v>
       </c>
     </row>
@@ -32975,7 +32902,7 @@
         <v>3471.316199994093</v>
       </c>
       <c r="E197">
-        <f>(C197/B197)</f>
+        <f t="shared" si="3"/>
         <v>131.48924999977626</v>
       </c>
     </row>
@@ -32993,7 +32920,7 @@
         <v>3505.3012500053455</v>
       </c>
       <c r="E198">
-        <f>(C198/B198)</f>
+        <f t="shared" si="3"/>
         <v>132.77656250020249</v>
       </c>
     </row>
@@ -33011,7 +32938,7 @@
         <v>3546.1169699952147</v>
       </c>
       <c r="E199">
-        <f>(C199/B199)</f>
+        <f t="shared" si="3"/>
         <v>134.32261249981875</v>
       </c>
     </row>
@@ -33029,7 +32956,7 @@
         <v>3543.1109970047264</v>
       </c>
       <c r="E200">
-        <f>(C200/B200)</f>
+        <f t="shared" si="3"/>
         <v>134.94481250018001</v>
       </c>
     </row>
@@ -33047,7 +32974,7 @@
         <v>3567.1122299956769</v>
       </c>
       <c r="E201">
-        <f>(C201/B201)</f>
+        <f t="shared" si="3"/>
         <v>135.11788749983626</v>
       </c>
     </row>
@@ -33065,7 +32992,7 @@
         <v>3560.8072127993373</v>
       </c>
       <c r="E202">
-        <f>(C202/B202)</f>
+        <f t="shared" si="3"/>
         <v>135.61879999997475</v>
       </c>
     </row>
@@ -33083,7 +33010,7 @@
         <v>3584.8485191999803</v>
       </c>
       <c r="E203">
-        <f>(C203/B203)</f>
+        <f t="shared" si="3"/>
         <v>136.53444999999925</v>
       </c>
     </row>
@@ -33101,7 +33028,7 @@
         <v>2716.3404799997807</v>
       </c>
       <c r="E204">
-        <f>(C204/B204)</f>
+        <f t="shared" si="3"/>
         <v>94.317377777770162</v>
       </c>
       <c r="F204">
@@ -33123,7 +33050,7 @@
         <v>2802.0061109999997</v>
       </c>
       <c r="E205">
-        <f>(C205/B205)</f>
+        <f t="shared" si="3"/>
         <v>96.988788888888891</v>
       </c>
     </row>
@@ -33141,7 +33068,7 @@
         <v>2817.1936005353928</v>
       </c>
       <c r="E206">
-        <f>(C206/B206)</f>
+        <f t="shared" si="3"/>
         <v>97.819222240812252</v>
       </c>
     </row>
@@ -33159,7 +33086,7 @@
         <v>2950.3494399948977</v>
       </c>
       <c r="E207">
-        <f>(C207/B207)</f>
+        <f t="shared" si="3"/>
         <v>102.44268888871173</v>
       </c>
     </row>
@@ -33177,7 +33104,7 @@
         <v>2981.386879994534</v>
       </c>
       <c r="E208">
-        <f>(C208/B208)</f>
+        <f t="shared" si="3"/>
         <v>103.52037777758798</v>
       </c>
     </row>
@@ -33195,7 +33122,7 @@
         <v>3012.4681600020267</v>
       </c>
       <c r="E209">
-        <f>(C209/B209)</f>
+        <f t="shared" si="3"/>
         <v>104.59958888895926</v>
       </c>
     </row>
@@ -33213,7 +33140,7 @@
         <v>3016.835519997403</v>
       </c>
       <c r="E210">
-        <f>(C210/B210)</f>
+        <f t="shared" si="3"/>
         <v>104.75123333324316</v>
       </c>
     </row>
@@ -33231,7 +33158,7 @@
         <v>3021.7225600033998</v>
       </c>
       <c r="E211">
-        <f>(C211/B211)</f>
+        <f t="shared" si="3"/>
         <v>104.92092222234027</v>
       </c>
     </row>
@@ -33249,7 +33176,7 @@
         <v>3025.7299199991394</v>
       </c>
       <c r="E212">
-        <f>(C212/B212)</f>
+        <f t="shared" si="3"/>
         <v>105.06006666663679</v>
       </c>
     </row>
@@ -33267,7 +33194,7 @@
         <v>3043.0329599999823</v>
       </c>
       <c r="E213">
-        <f>(C213/B213)</f>
+        <f t="shared" si="3"/>
         <v>105.66086666666605</v>
       </c>
     </row>
@@ -33285,7 +33212,7 @@
         <v>3032.77774</v>
       </c>
       <c r="E214">
-        <f>(C214/B214)</f>
+        <f t="shared" si="3"/>
         <v>108.70171111111111</v>
       </c>
     </row>
@@ -33303,7 +33230,7 @@
         <v>3147.6179199991748</v>
       </c>
       <c r="E215">
-        <f>(C215/B215)</f>
+        <f t="shared" si="3"/>
         <v>109.29228888886024</v>
       </c>
     </row>
@@ -33321,7 +33248,7 @@
         <v>3051.53739</v>
       </c>
       <c r="E216">
-        <f>(C216/B216)</f>
+        <f t="shared" si="3"/>
         <v>109.3741</v>
       </c>
     </row>
@@ -33339,7 +33266,7 @@
         <v>3184.2675199965015</v>
       </c>
       <c r="E217">
-        <f>(C217/B217)</f>
+        <f t="shared" si="3"/>
         <v>110.56484444432297</v>
       </c>
     </row>
@@ -33357,7 +33284,7 @@
         <v>3256.1974400014146</v>
       </c>
       <c r="E218">
-        <f>(C218/B218)</f>
+        <f t="shared" si="3"/>
         <v>113.06241111116022</v>
       </c>
     </row>
@@ -33375,7 +33302,7 @@
         <v>3260.646079998698</v>
       </c>
       <c r="E219">
-        <f>(C219/B219)</f>
+        <f t="shared" si="3"/>
         <v>113.21687777773256</v>
       </c>
     </row>
@@ -33393,7 +33320,7 @@
         <v>3270.3795199980959</v>
       </c>
       <c r="E220">
-        <f>(C220/B220)</f>
+        <f t="shared" si="3"/>
         <v>113.55484444437833</v>
       </c>
     </row>
@@ -33411,7 +33338,7 @@
         <v>3380.2507199972742</v>
       </c>
       <c r="E221">
-        <f>(C221/B221)</f>
+        <f t="shared" si="3"/>
         <v>113.81315555546378</v>
       </c>
     </row>
@@ -33429,7 +33356,7 @@
         <v>3201.6564400000002</v>
       </c>
       <c r="E222">
-        <f>(C222/B222)</f>
+        <f t="shared" si="3"/>
         <v>114.75471111111112</v>
       </c>
     </row>
@@ -33447,7 +33374,7 @@
         <v>3423.3170399998908</v>
       </c>
       <c r="E223">
-        <f>(C223/B223)</f>
+        <f t="shared" si="3"/>
         <v>115.26319999999633</v>
       </c>
     </row>
@@ -33465,7 +33392,7 @@
         <v>3464.3093099966795</v>
       </c>
       <c r="E224">
-        <f>(C224/B224)</f>
+        <f t="shared" si="3"/>
         <v>116.64341111099932</v>
       </c>
     </row>
@@ -33483,7 +33410,7 @@
         <v>3382.0358400000259</v>
       </c>
       <c r="E225">
-        <f>(C225/B225)</f>
+        <f t="shared" si="3"/>
         <v>117.43180000000091</v>
       </c>
     </row>
@@ -33501,7 +33428,7 @@
         <v>3412.9958400037158</v>
       </c>
       <c r="E226">
-        <f>(C226/B226)</f>
+        <f t="shared" si="3"/>
         <v>118.506800000129</v>
       </c>
     </row>
@@ -33519,7 +33446,7 @@
         <v>3428.1257600057857</v>
       </c>
       <c r="E227">
-        <f>(C227/B227)</f>
+        <f t="shared" si="3"/>
         <v>119.03214444464533</v>
       </c>
     </row>
@@ -33537,7 +33464,7 @@
         <v>3479.0598400053568</v>
       </c>
       <c r="E228">
-        <f>(C228/B228)</f>
+        <f t="shared" si="3"/>
         <v>120.80068888907489</v>
       </c>
     </row>
@@ -33555,7 +33482,7 @@
         <v>3506.8556800019014</v>
       </c>
       <c r="E229">
-        <f>(C229/B229)</f>
+        <f t="shared" si="3"/>
         <v>121.76582222228824</v>
       </c>
     </row>
@@ -33573,7 +33500,7 @@
         <v>3420.3645399946249</v>
       </c>
       <c r="E230">
-        <f>(C230/B230)</f>
+        <f t="shared" si="3"/>
         <v>122.59371111091845</v>
       </c>
     </row>
@@ -33591,7 +33518,7 @@
         <v>3434.5008500007689</v>
       </c>
       <c r="E231">
-        <f>(C231/B231)</f>
+        <f t="shared" si="3"/>
         <v>123.10038888891644</v>
       </c>
     </row>
@@ -33609,7 +33536,7 @@
         <v>3665.0308200027225</v>
       </c>
       <c r="E232">
-        <f>(C232/B232)</f>
+        <f t="shared" si="3"/>
         <v>123.40171111120279</v>
       </c>
     </row>
@@ -33627,7 +33554,7 @@
         <v>3692.8541099929148</v>
       </c>
       <c r="E233">
-        <f>(C233/B233)</f>
+        <f t="shared" si="3"/>
         <v>124.33852222198367</v>
       </c>
     </row>
@@ -33645,7 +33572,7 @@
         <v>3779.021730000386</v>
       </c>
       <c r="E234">
-        <f>(C234/B234)</f>
+        <f t="shared" si="3"/>
         <v>127.23978888890188</v>
       </c>
     </row>
@@ -33663,7 +33590,7 @@
         <v>3606.8484499955953</v>
       </c>
       <c r="E235">
-        <f>(C235/B235)</f>
+        <f t="shared" si="3"/>
         <v>129.27772222206434</v>
       </c>
     </row>
@@ -33681,7 +33608,7 @@
         <v>3714.9962899977249</v>
       </c>
       <c r="E236">
-        <f>(C236/B236)</f>
+        <f t="shared" si="3"/>
         <v>133.15398888880733</v>
       </c>
     </row>
@@ -33699,7 +33626,7 @@
         <v>3969.5086199895754</v>
       </c>
       <c r="E237">
-        <f>(C237/B237)</f>
+        <f t="shared" si="3"/>
         <v>133.65348888853791</v>
       </c>
     </row>
@@ -33717,7 +33644,7 @@
         <v>4016.5646399982506</v>
       </c>
       <c r="E238">
-        <f>(C238/B238)</f>
+        <f t="shared" si="3"/>
         <v>135.23786666660777</v>
       </c>
     </row>
@@ -33735,7 +33662,7 @@
         <v>4047.9304799991951</v>
       </c>
       <c r="E239">
-        <f>(C239/B239)</f>
+        <f t="shared" si="3"/>
         <v>136.29395555552844</v>
       </c>
     </row>
@@ -33753,7 +33680,7 @@
         <v>3874.2783199970304</v>
       </c>
       <c r="E240">
-        <f>(C240/B240)</f>
+        <f t="shared" si="3"/>
         <v>138.86302222211577</v>
       </c>
     </row>
@@ -33771,7 +33698,7 @@
         <v>3899.7559800004406</v>
       </c>
       <c r="E241">
-        <f>(C241/B241)</f>
+        <f t="shared" si="3"/>
         <v>139.77620000001579</v>
       </c>
     </row>
@@ -33789,7 +33716,7 @@
         <v>4145.8318440001322</v>
       </c>
       <c r="E242">
-        <f>(C242/B242)</f>
+        <f t="shared" si="3"/>
         <v>143.50404444444902</v>
       </c>
     </row>
@@ -33807,7 +33734,7 @@
         <v>4146.0982739969058</v>
       </c>
       <c r="E243">
-        <f>(C243/B243)</f>
+        <f t="shared" si="3"/>
         <v>143.51326666655956</v>
       </c>
     </row>
@@ -33825,7 +33752,7 @@
         <v>4048.9496800026259</v>
       </c>
       <c r="E244">
-        <f>(C244/B244)</f>
+        <f t="shared" si="3"/>
         <v>145.12364444453857</v>
       </c>
     </row>
@@ -33843,7 +33770,7 @@
         <v>4239.113599999836</v>
       </c>
       <c r="E245">
-        <f>(C245/B245)</f>
+        <f t="shared" si="3"/>
         <v>151.93955555554965</v>
       </c>
     </row>
@@ -33861,7 +33788,7 @@
         <v>4479.3893639958687</v>
       </c>
       <c r="E246">
-        <f>(C246/B246)</f>
+        <f t="shared" si="3"/>
         <v>155.04982222207923</v>
       </c>
     </row>
@@ -33879,7 +33806,7 @@
         <v>2809.8056000045599</v>
       </c>
       <c r="E247">
-        <f>(C247/B247)</f>
+        <f t="shared" si="3"/>
         <v>90.303730000000002</v>
       </c>
       <c r="F247">
@@ -33901,7 +33828,7 @@
         <v>2770.8434999999554</v>
       </c>
       <c r="E248">
-        <f>(C248/B248)</f>
+        <f t="shared" si="3"/>
         <v>92.361449999998513</v>
       </c>
     </row>
@@ -33919,7 +33846,7 @@
         <v>2838.5898000051384</v>
       </c>
       <c r="E249">
-        <f>(C249/B249)</f>
+        <f t="shared" si="3"/>
         <v>94.61966000017128</v>
       </c>
     </row>
@@ -33937,7 +33864,7 @@
         <v>2852.1129000037035</v>
       </c>
       <c r="E250">
-        <f>(C250/B250)</f>
+        <f t="shared" si="3"/>
         <v>95.070430000123451</v>
       </c>
     </row>
@@ -33955,7 +33882,7 @@
         <v>2853.0333000053361</v>
       </c>
       <c r="E251">
-        <f>(C251/B251)</f>
+        <f t="shared" si="3"/>
         <v>95.101110000177869</v>
       </c>
     </row>
@@ -33973,7 +33900,7 @@
         <v>2890.8687000000555</v>
       </c>
       <c r="E252">
-        <f>(C252/B252)</f>
+        <f t="shared" si="3"/>
         <v>96.362290000001849</v>
       </c>
     </row>
@@ -33991,7 +33918,7 @@
         <v>2907.2880000021541</v>
       </c>
       <c r="E253">
-        <f>(C253/B253)</f>
+        <f t="shared" si="3"/>
         <v>96.909600000071805</v>
       </c>
     </row>
@@ -34009,7 +33936,7 @@
         <v>2940.0786000078369</v>
       </c>
       <c r="E254">
-        <f>(C254/B254)</f>
+        <f t="shared" si="3"/>
         <v>98.002620000261231</v>
       </c>
     </row>
@@ -34027,7 +33954,7 @@
         <v>2941.314899991994</v>
       </c>
       <c r="E255">
-        <f>(C255/B255)</f>
+        <f t="shared" si="3"/>
         <v>98.043829999733134</v>
       </c>
     </row>
@@ -34045,7 +33972,7 @@
         <v>2945.6285999985994</v>
       </c>
       <c r="E256">
-        <f>(C256/B256)</f>
+        <f t="shared" si="3"/>
         <v>98.187619999953313</v>
       </c>
     </row>
@@ -34063,7 +33990,7 @@
         <v>2964.3758999971201</v>
       </c>
       <c r="E257">
-        <f>(C257/B257)</f>
+        <f t="shared" si="3"/>
         <v>98.877170000000007</v>
       </c>
     </row>
@@ -34081,7 +34008,7 @@
         <v>2967.71120000056</v>
       </c>
       <c r="E258">
-        <f>(C258/B258)</f>
+        <f t="shared" ref="E258:E315" si="4">(C258/B258)</f>
         <v>98.922539999999998</v>
       </c>
       <c r="V258" s="1"/>
@@ -34100,7 +34027,7 @@
         <v>2969.0480999925057</v>
       </c>
       <c r="E259">
-        <f>(C259/B259)</f>
+        <f t="shared" si="4"/>
         <v>98.968269999750191</v>
       </c>
     </row>
@@ -34118,7 +34045,7 @@
         <v>2981.4976000002298</v>
       </c>
       <c r="E260">
-        <f>(C260/B260)</f>
+        <f t="shared" si="4"/>
         <v>99.065629998221993</v>
       </c>
     </row>
@@ -34136,7 +34063,7 @@
         <v>3022.7708999917299</v>
       </c>
       <c r="E261">
-        <f>(C261/B261)</f>
+        <f t="shared" si="4"/>
         <v>100.48051000000001</v>
       </c>
     </row>
@@ -34154,7 +34081,7 @@
         <v>3025.6541999951883</v>
       </c>
       <c r="E262">
-        <f>(C262/B262)</f>
+        <f t="shared" si="4"/>
         <v>100.85513999983961</v>
       </c>
     </row>
@@ -34172,7 +34099,7 @@
         <v>3141.1511999995901</v>
       </c>
       <c r="E263">
-        <f>(C263/B263)</f>
+        <f t="shared" si="4"/>
         <v>104.7906</v>
       </c>
     </row>
@@ -34190,7 +34117,7 @@
         <v>3186.0633000069365</v>
       </c>
       <c r="E264">
-        <f>(C264/B264)</f>
+        <f t="shared" si="4"/>
         <v>106.20211000023122</v>
       </c>
     </row>
@@ -34208,7 +34135,7 @@
         <v>3318.0462000018451</v>
       </c>
       <c r="E265">
-        <f>(C265/B265)</f>
+        <f t="shared" si="4"/>
         <v>110.6015400000615</v>
       </c>
     </row>
@@ -34226,7 +34153,7 @@
         <v>3353.770200003054</v>
       </c>
       <c r="E266">
-        <f>(C266/B266)</f>
+        <f t="shared" si="4"/>
         <v>111.7923400001018</v>
       </c>
     </row>
@@ -34244,7 +34171,7 @@
         <v>3476.574600001185</v>
       </c>
       <c r="E267">
-        <f>(C267/B267)</f>
+        <f t="shared" si="4"/>
         <v>115.8858200000395</v>
       </c>
     </row>
@@ -34262,7 +34189,7 @@
         <v>3482.6873999991208</v>
       </c>
       <c r="E268">
-        <f>(C268/B268)</f>
+        <f t="shared" si="4"/>
         <v>116.0895799999707</v>
       </c>
     </row>
@@ -34280,7 +34207,7 @@
         <v>3562.7817000004143</v>
       </c>
       <c r="E269">
-        <f>(C269/B269)</f>
+        <f t="shared" si="4"/>
         <v>118.75939000001381</v>
       </c>
     </row>
@@ -34298,7 +34225,7 @@
         <v>3545.8686999996899</v>
       </c>
       <c r="E270">
-        <f>(C270/B270)</f>
+        <f t="shared" si="4"/>
         <v>119.96228999998951</v>
       </c>
     </row>
@@ -34316,7 +34243,7 @@
         <v>3603.6096000061648</v>
       </c>
       <c r="E271">
-        <f>(C271/B271)</f>
+        <f t="shared" si="4"/>
         <v>120.1203200002055</v>
       </c>
     </row>
@@ -34334,7 +34261,7 @@
         <v>3605.4488999980081</v>
       </c>
       <c r="E272">
-        <f>(C272/B272)</f>
+        <f t="shared" si="4"/>
         <v>120.18162999993361</v>
       </c>
     </row>
@@ -34352,7 +34279,7 @@
         <v>3608.7941999976479</v>
       </c>
       <c r="E273">
-        <f>(C273/B273)</f>
+        <f t="shared" si="4"/>
         <v>120.29313999992159</v>
       </c>
     </row>
@@ -34370,7 +34297,7 @@
         <v>3624.8235000020941</v>
       </c>
       <c r="E274">
-        <f>(C274/B274)</f>
+        <f t="shared" si="4"/>
         <v>120.8274500000698</v>
       </c>
     </row>
@@ -34388,7 +34315,7 @@
         <v>3696.4047000037681</v>
       </c>
       <c r="E275">
-        <f>(C275/B275)</f>
+        <f t="shared" si="4"/>
         <v>123.2134900001256</v>
       </c>
     </row>
@@ -34406,7 +34333,7 @@
         <v>3755.9237999994357</v>
       </c>
       <c r="E276">
-        <f>(C276/B276)</f>
+        <f t="shared" si="4"/>
         <v>125.19745999998119</v>
       </c>
     </row>
@@ -34424,7 +34351,7 @@
         <v>3761.191199999304</v>
       </c>
       <c r="E277">
-        <f>(C277/B277)</f>
+        <f t="shared" si="4"/>
         <v>125.3730399999768</v>
       </c>
     </row>
@@ -34442,7 +34369,7 @@
         <v>3924.920999997993</v>
       </c>
       <c r="E278">
-        <f>(C278/B278)</f>
+        <f t="shared" si="4"/>
         <v>130.8306999999331</v>
       </c>
     </row>
@@ -34460,7 +34387,7 @@
         <v>4036.8801000004169</v>
       </c>
       <c r="E279">
-        <f>(C279/B279)</f>
+        <f t="shared" si="4"/>
         <v>134.5626700000139</v>
       </c>
     </row>
@@ -34478,7 +34405,7 @@
         <v>4046.2700999923982</v>
       </c>
       <c r="E280">
-        <f>(C280/B280)</f>
+        <f t="shared" si="4"/>
         <v>134.87566999974661</v>
       </c>
     </row>
@@ -34496,7 +34423,7 @@
         <v>4166.9261999977625</v>
       </c>
       <c r="E281">
-        <f>(C281/B281)</f>
+        <f t="shared" si="4"/>
         <v>138.89753999992541</v>
       </c>
     </row>
@@ -34514,7 +34441,7 @@
         <v>4186.5623999965474</v>
       </c>
       <c r="E282">
-        <f>(C282/B282)</f>
+        <f t="shared" si="4"/>
         <v>139.55207999988491</v>
       </c>
     </row>
@@ -34532,7 +34459,7 @@
         <v>2958.9243999999999</v>
       </c>
       <c r="E283">
-        <f>(C283/B283)</f>
+        <f t="shared" si="4"/>
         <v>89.66439996363637</v>
       </c>
       <c r="F283">
@@ -34554,7 +34481,7 @@
         <v>2996.4216000043962</v>
       </c>
       <c r="E284">
-        <f>(C284/B284)</f>
+        <f t="shared" si="4"/>
         <v>90.800654545587761</v>
       </c>
     </row>
@@ -34572,7 +34499,7 @@
         <v>3073.3337999990908</v>
       </c>
       <c r="E285">
-        <f>(C285/B285)</f>
+        <f t="shared" si="4"/>
         <v>93.131327272699721</v>
       </c>
     </row>
@@ -34590,7 +34517,7 @@
         <v>3090.8871000010563</v>
       </c>
       <c r="E286">
-        <f>(C286/B286)</f>
+        <f t="shared" si="4"/>
         <v>93.663245454577464</v>
       </c>
     </row>
@@ -34608,7 +34535,7 @@
         <v>3100.1318999999521</v>
       </c>
       <c r="E287">
-        <f>(C287/B287)</f>
+        <f t="shared" si="4"/>
         <v>93.943390909089445</v>
       </c>
     </row>
@@ -34626,7 +34553,7 @@
         <v>3162.4178999943501</v>
       </c>
       <c r="E288">
-        <f>(C288/B288)</f>
+        <f t="shared" si="4"/>
         <v>95.850772727272727</v>
       </c>
     </row>
@@ -34644,7 +34571,7 @@
         <v>3389.0010000012298</v>
       </c>
       <c r="E289">
-        <f>(C289/B289)</f>
+        <f t="shared" si="4"/>
         <v>99.969727272764445</v>
       </c>
     </row>
@@ -34662,7 +34589,7 @@
         <v>3533.0319000058798</v>
       </c>
       <c r="E290">
-        <f>(C290/B290)</f>
+        <f t="shared" si="4"/>
         <v>107.06157272745091</v>
       </c>
     </row>
@@ -34680,7 +34607,7 @@
         <v>3606.5706000044875</v>
       </c>
       <c r="E291">
-        <f>(C291/B291)</f>
+        <f t="shared" si="4"/>
         <v>109.29001818195417</v>
       </c>
     </row>
@@ -34698,7 +34625,7 @@
         <v>3692.6964000012958</v>
       </c>
       <c r="E292">
-        <f>(C292/B292)</f>
+        <f t="shared" si="4"/>
         <v>111.89989090913018</v>
       </c>
     </row>
@@ -34716,7 +34643,7 @@
         <v>3845.5514999986917</v>
       </c>
       <c r="E293">
-        <f>(C293/B293)</f>
+        <f t="shared" si="4"/>
         <v>116.53186363632399</v>
       </c>
     </row>
@@ -34734,7 +34661,7 @@
         <v>3914.7300000022383</v>
       </c>
       <c r="E294">
-        <f>(C294/B294)</f>
+        <f t="shared" si="4"/>
         <v>118.62818181824964</v>
       </c>
     </row>
@@ -34752,7 +34679,7 @@
         <v>2985.3514999990998</v>
       </c>
       <c r="E295">
-        <f>(C295/B295)</f>
+        <f t="shared" si="4"/>
         <v>82.573691666666676</v>
       </c>
       <c r="F295">
@@ -34774,7 +34701,7 @@
         <v>3019.1334000010111</v>
       </c>
       <c r="E296">
-        <f>(C296/B296)</f>
+        <f t="shared" si="4"/>
         <v>83.86481666669475</v>
       </c>
     </row>
@@ -34792,7 +34719,7 @@
         <v>3280.6391999984035</v>
       </c>
       <c r="E297">
-        <f>(C297/B297)</f>
+        <f t="shared" si="4"/>
         <v>91.128866666622329</v>
       </c>
     </row>
@@ -34810,7 +34737,7 @@
         <v>3297.3191999972187</v>
       </c>
       <c r="E298">
-        <f>(C298/B298)</f>
+        <f t="shared" si="4"/>
         <v>91.592199999922741</v>
       </c>
     </row>
@@ -34828,7 +34755,7 @@
         <v>3351.6364000077001</v>
       </c>
       <c r="E299">
-        <f>(C299/B299)</f>
+        <f t="shared" si="4"/>
         <v>92.82323333354725</v>
       </c>
     </row>
@@ -34846,7 +34773,7 @@
         <v>3547.4298000081026</v>
       </c>
       <c r="E300">
-        <f>(C300/B300)</f>
+        <f t="shared" si="4"/>
         <v>98.539716666891749</v>
       </c>
     </row>
@@ -34864,7 +34791,7 @@
         <v>3621.977999999217</v>
       </c>
       <c r="E301">
-        <f>(C301/B301)</f>
+        <f t="shared" si="4"/>
         <v>100.61049999997825</v>
       </c>
     </row>
@@ -34882,7 +34809,7 @@
         <v>3966.2435999998715</v>
       </c>
       <c r="E302">
-        <f>(C302/B302)</f>
+        <f t="shared" si="4"/>
         <v>110.17343333332975</v>
       </c>
     </row>
@@ -34900,7 +34827,7 @@
         <v>2909.0568000028725</v>
       </c>
       <c r="E303">
-        <f>(C303/B303)</f>
+        <f t="shared" si="4"/>
         <v>74.591200000073655</v>
       </c>
       <c r="F303">
@@ -34922,7 +34849,7 @@
         <v>3139.7196000034469</v>
       </c>
       <c r="E304">
-        <f>(C304/B304)</f>
+        <f t="shared" si="4"/>
         <v>80.505630769319154</v>
       </c>
     </row>
@@ -34940,7 +34867,7 @@
         <v>3199.1525999965102</v>
       </c>
       <c r="E305">
-        <f>(C305/B305)</f>
+        <f t="shared" si="4"/>
         <v>81.798784615295077</v>
       </c>
     </row>
@@ -34958,7 +34885,7 @@
         <v>3219.1698000034398</v>
       </c>
       <c r="E306">
-        <f>(C306/B306)</f>
+        <f t="shared" si="4"/>
         <v>82.600100000000012</v>
       </c>
     </row>
@@ -34976,7 +34903,7 @@
         <v>3268.9046999985303</v>
       </c>
       <c r="E307">
-        <f>(C307/B307)</f>
+        <f t="shared" si="4"/>
         <v>83.818069230731538</v>
       </c>
     </row>
@@ -34994,7 +34921,7 @@
         <v>3768.1580999960729</v>
       </c>
       <c r="E308">
-        <f>(C308/B308)</f>
+        <f t="shared" si="4"/>
         <v>96.619438461437767</v>
       </c>
     </row>
@@ -35012,7 +34939,7 @@
         <v>3325.41689999963</v>
       </c>
       <c r="E309">
-        <f>(C309/B309)</f>
+        <f t="shared" si="4"/>
         <v>79.059399999999997</v>
       </c>
       <c r="F309">
@@ -35034,7 +34961,7 @@
         <v>3342.5403999952</v>
       </c>
       <c r="E310">
-        <f>(C310/B310)</f>
+        <f t="shared" si="4"/>
         <v>79.346199999885656</v>
       </c>
     </row>
@@ -35052,7 +34979,7 @@
         <v>3498.86730000435</v>
       </c>
       <c r="E311">
-        <f>(C311/B311)</f>
+        <f t="shared" si="4"/>
         <v>77.752606666763327</v>
       </c>
       <c r="F311">
@@ -35074,7 +35001,7 @@
         <v>4057.8345999920598</v>
       </c>
       <c r="E312">
-        <f>(C312/B312)</f>
+        <f t="shared" si="4"/>
         <v>89.285213333156804</v>
       </c>
     </row>
@@ -35092,7 +35019,7 @@
         <v>3482.21299999859</v>
       </c>
       <c r="E313">
-        <f>(C313/B313)</f>
+        <f t="shared" si="4"/>
         <v>69.086650000000006</v>
       </c>
       <c r="F313">
@@ -35114,7 +35041,7 @@
         <v>3786.5364999943099</v>
       </c>
       <c r="E314">
-        <f>(C314/B314)</f>
+        <f t="shared" si="4"/>
         <v>66.422015789473676</v>
       </c>
       <c r="F314">
@@ -35136,7 +35063,7 @@
         <v>4215.3331000001299</v>
       </c>
       <c r="E315">
-        <f>(C315/B315)</f>
+        <f t="shared" si="4"/>
         <v>66.941795238097328</v>
       </c>
       <c r="F315">
@@ -35153,11 +35080,11 @@
         <v>1405.777700000044</v>
       </c>
       <c r="D316">
-        <f t="shared" ref="D316:E316" si="0">MAX(D2:D315)</f>
+        <f t="shared" ref="D316:E316" si="5">MAX(D2:D315)</f>
         <v>4479.3893639958687</v>
       </c>
       <c r="E316">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>716.73120000050403</v>
       </c>
     </row>
@@ -35170,11 +35097,11 @@
         <v>603.041100000337</v>
       </c>
       <c r="D317">
-        <f t="shared" ref="D317:E317" si="1">MIN(D2:D315)</f>
+        <f t="shared" ref="D317:E317" si="6">MIN(D2:D315)</f>
         <v>1980.1662299999998</v>
       </c>
       <c r="E317">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>66.422015789473676</v>
       </c>
     </row>
@@ -35194,8 +35121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED9FE13A-DACE-47D6-A8D1-9B48DFC775A1}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>